<commit_message>
chatbot for cyan system manager
</commit_message>
<xml_diff>
--- a/WG/Shared/cleaning_plan.xlsx
+++ b/WG/Shared/cleaning_plan.xlsx
@@ -38,22 +38,22 @@
     <t>Mara</t>
   </si>
   <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>Bathrooms</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Anarchy</t>
+  </si>
+  <si>
     <t>Floor</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>Vacation</t>
-  </si>
-  <si>
-    <t>Bathrooms</t>
-  </si>
-  <si>
-    <t>Kitchen</t>
-  </si>
-  <si>
-    <t>Anarchy</t>
   </si>
   <si>
     <t>Hallway's floor</t>
@@ -529,45 +529,45 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="3">
-        <v>45341</v>
+        <v>45348</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="3">
-        <v>45348</v>
+        <v>45355</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -575,30 +575,30 @@
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="3">
-        <v>45355</v>
+        <v>45362</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1">
       <c r="A5" s="3">
-        <v>45362</v>
+        <v>45369</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
@@ -607,13 +607,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>7</v>
@@ -621,45 +621,45 @@
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="3">
-        <v>45369</v>
+        <v>45376</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1">
       <c r="A7" s="3">
-        <v>45376</v>
+        <v>45383</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>12</v>
@@ -667,114 +667,114 @@
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1">
       <c r="A8" s="3">
-        <v>45383</v>
+        <v>45390</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1">
       <c r="A9" s="3">
-        <v>45390</v>
+        <v>45397</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1">
       <c r="A10" s="3">
-        <v>45397</v>
+        <v>45404</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1">
       <c r="A11" s="3">
-        <v>45404</v>
+        <v>45411</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1">
       <c r="A12" s="3">
-        <v>45411</v>
+        <v>45418</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>10</v>
@@ -782,94 +782,94 @@
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1">
       <c r="A13" s="3">
-        <v>45418</v>
+        <v>45425</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1">
       <c r="A14" s="3">
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1">
       <c r="A15" s="3">
-        <v>45432</v>
+        <v>45439</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1">
       <c r="A16" s="3">
-        <v>45439</v>
+        <v>45446</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1"/>
@@ -994,16 +994,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1">

</xml_diff>